<commit_message>
Update USSC Transmittal(Replacement printer) 1-10-23.xlsx
</commit_message>
<xml_diff>
--- a/USSC Transmittal(Replacement printer) 1-10-23.xlsx
+++ b/USSC Transmittal(Replacement printer) 1-10-23.xlsx
@@ -156,9 +156,6 @@
     <t>Replacement Printer</t>
   </si>
   <si>
-    <t>2 Units</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -170,7 +167,6 @@
       </rPr>
       <t xml:space="preserve">Javelin DNA PRO 
 NU18107045
-NU18107053
 </t>
     </r>
     <r>
@@ -184,6 +180,9 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>1 Unit</t>
   </si>
 </sst>
 </file>
@@ -909,6 +908,36 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -926,36 +955,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1688,16 +1687,16 @@
     <row r="3" spans="1:20" ht="27.75">
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="70"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="80"/>
     </row>
     <row r="4" spans="1:20" ht="27.75">
       <c r="A4" s="20"/>
@@ -1724,77 +1723,77 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="68" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="72"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="82"/>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1">
-      <c r="A7" s="77"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="11"/>
       <c r="C7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="72"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="82"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="77"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="11"/>
       <c r="C8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D8" s="69">
         <v>42836</v>
       </c>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="75"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="71"/>
       <c r="M8" s="11"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="77"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="11"/>
       <c r="C9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="75"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
@@ -1804,7 +1803,7 @@
       <c r="S9" s="11"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="77"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="11"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
@@ -1828,13 +1827,13 @@
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="28"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="79"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="73"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="53"/>
@@ -1849,15 +1848,15 @@
       <c r="C12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="80" t="s">
+      <c r="D12" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="82"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="76"/>
       <c r="O12" s="54"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1">
@@ -1885,9 +1884,9 @@
       <c r="I14" s="36"/>
       <c r="J14" s="56"/>
       <c r="O14" s="54"/>
-      <c r="R14" s="67"/>
-      <c r="S14" s="67"/>
-      <c r="T14" s="67"/>
+      <c r="R14" s="77"/>
+      <c r="S14" s="77"/>
+      <c r="T14" s="77"/>
     </row>
     <row r="15" spans="1:20" ht="22.5" customHeight="1">
       <c r="A15" s="27"/>
@@ -2377,14 +2376,14 @@
     <row r="48" spans="1:15" ht="27.75">
       <c r="A48" s="49"/>
       <c r="B48" s="11"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="68"/>
-      <c r="J48" s="68"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="78"/>
     </row>
     <row r="49" spans="1:17">
       <c r="A49" s="50"/>
@@ -2433,10 +2432,10 @@
       <c r="H52" s="50"/>
       <c r="I52" s="50"/>
       <c r="J52" s="50"/>
-      <c r="N52" s="76"/>
-      <c r="O52" s="76"/>
-      <c r="P52" s="76"/>
-      <c r="Q52" s="76"/>
+      <c r="N52" s="67"/>
+      <c r="O52" s="67"/>
+      <c r="P52" s="67"/>
+      <c r="Q52" s="67"/>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="50"/>
@@ -2694,11 +2693,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="N52:Q52"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D12:J12"/>
     <mergeCell ref="R14:T14"/>
     <mergeCell ref="C48:J48"/>
     <mergeCell ref="C3:J3"/>
@@ -2706,6 +2700,11 @@
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="N52:Q52"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D12:J12"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2722,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:E31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2844,10 +2843,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="83" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="83" t="s">
-        <v>34</v>
       </c>
       <c r="C15" s="84"/>
       <c r="D15" s="84"/>

</xml_diff>